<commit_message>
benerin fitur import dan rubah dashboard
</commit_message>
<xml_diff>
--- a/public/templates/template_karyawan.xlsx
+++ b/public/templates/template_karyawan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\KSP-Casual\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E7E12A7-C976-4603-9BA5-F595C1E61E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD644146-2B8F-40F5-8D0B-B8D1C23DC120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="1680" windowWidth="14670" windowHeight="8325" xr2:uid="{7EF3EB6D-84D0-4EF5-A22C-33E296879379}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7EF3EB6D-84D0-4EF5-A22C-33E296879379}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="List" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>nomor_karyawan</t>
   </si>
@@ -63,13 +64,103 @@
     <t>3600987654321001</t>
   </si>
   <si>
-    <t>1234567891011122</t>
-  </si>
-  <si>
     <t>3600987654321002</t>
   </si>
   <si>
-    <t>finance</t>
+    <t>Aktif</t>
+  </si>
+  <si>
+    <t>3600987689764283</t>
+  </si>
+  <si>
+    <t>bandung</t>
+  </si>
+  <si>
+    <t>1234567891112131</t>
+  </si>
+  <si>
+    <t>3600987654321201</t>
+  </si>
+  <si>
+    <t>Nonaktif</t>
+  </si>
+  <si>
+    <t>1234567891011123</t>
+  </si>
+  <si>
+    <t>0004</t>
+  </si>
+  <si>
+    <t>accounting</t>
+  </si>
+  <si>
+    <t>budi karyawan</t>
+  </si>
+  <si>
+    <t>Building Management &amp; Office Rent</t>
+  </si>
+  <si>
+    <t>Engineering Planning</t>
+  </si>
+  <si>
+    <t>Business Development</t>
+  </si>
+  <si>
+    <t>Corporate Secretary</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Executive Cheff</t>
+  </si>
+  <si>
+    <t>Executive Marketing &amp; Sales Hotel</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Food &amp; Beverage</t>
+  </si>
+  <si>
+    <t>Front Office</t>
+  </si>
+  <si>
+    <t>Golf &amp; Sport Center Manager</t>
+  </si>
+  <si>
+    <t>Housekeeping</t>
+  </si>
+  <si>
+    <t>Human Capital</t>
+  </si>
+  <si>
+    <t>Industrial Estate &amp; Housing</t>
+  </si>
+  <si>
+    <t>Internal Audit</t>
+  </si>
+  <si>
+    <t>IT &amp; Management System</t>
+  </si>
+  <si>
+    <t>legal &amp; Compliance</t>
+  </si>
+  <si>
+    <t>Marketing Industrial Estate &amp; Housing</t>
+  </si>
+  <si>
+    <t>Procurement</t>
+  </si>
+  <si>
+    <t>Project Control</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
+  </si>
+  <si>
+    <t>Security Fire &amp; SHE Manager</t>
   </si>
 </sst>
 </file>
@@ -430,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0760BE40-4028-484D-B082-D95BD47DB75F}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,9 +532,9 @@
     <col min="1" max="1" width="18.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -487,20 +578,203 @@
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{456E4AB2-E99D-4011-A1EF-9FFD26BA5C12}">
+          <x14:formula1>
+            <xm:f>List!$A$1:$A$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F035814F-2599-4C4B-A26A-5DE9CA7D11D4}">
+          <x14:formula1>
+            <xm:f>List!$B$1:$B$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D00EEC-34BE-4B7E-A416-65D663EF2330}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>